<commit_message>
readme and s2t updated
</commit_message>
<xml_diff>
--- a/s2t/s2t_all_platforms.xlsx
+++ b/s2t/s2t_all_platforms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Рабочий стол\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dbt_mcdm_challenge\s2t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EDAA60-2459-4D40-B7DD-72438E00BD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E580771B-56E1-4A2C-946C-A63A6BEC8456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{703711C0-3DA0-4B2F-B28D-CBD94DE6FB1B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>mcdm_field_name</t>
   </si>
@@ -127,13 +127,28 @@
   </si>
   <si>
     <t>video_views</t>
+  </si>
+  <si>
+    <t>TWITTER</t>
+  </si>
+  <si>
+    <t>url_clicks</t>
+  </si>
+  <si>
+    <t>video_total_views</t>
+  </si>
+  <si>
+    <t>MCDM</t>
+  </si>
+  <si>
+    <t>Field</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +164,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,16 +205,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,9 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE87F15-C7FC-49F2-854F-A30A63281223}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -516,398 +589,601 @@
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="str">
-        <f>C2&amp;" as "&amp;A2&amp;","</f>
+      <c r="D3" s="2" t="str">
+        <f t="shared" ref="D3:D27" si="0">C3&amp;" as "&amp;A3&amp;","</f>
         <v>ad_id as ad_id,</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>E3&amp;" as "&amp;A3&amp;","</f>
+        <v>NULL as ad_id,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f>C3&amp;" as "&amp;A3&amp;","</f>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as add_to_cart,</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f t="shared" ref="F4:F27" si="1">E4&amp;" as "&amp;A4&amp;","</f>
+        <v>0 as add_to_cart,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>C4&amp;" as "&amp;A4&amp;","</f>
-        <v>adset_id as adset_id,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>adset_id as adset_id,</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>NULL as adset_id,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f>C5&amp;" as "&amp;A5&amp;","</f>
-        <v>campaign_id as campaign_id,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>campaign_id as campaign_id,</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>campaign_id as campaign_id,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <f>C6&amp;" as "&amp;A6&amp;","</f>
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>BING as channel,</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>TWITTER as channel,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="str">
-        <f>C7&amp;" as "&amp;A7&amp;","</f>
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>clicks as clicks,</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>clicks as clicks,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f>C8&amp;" as "&amp;A8&amp;","</f>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as comments,</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>comments as comments,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2" t="str">
-        <f>C9&amp;" as "&amp;A9&amp;","</f>
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>NULL as creative_id,</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>NULL as creative_id,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f>C10&amp;" as "&amp;A10&amp;","</f>
+      <c r="D11" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>date as date,</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>date as date,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f>C11&amp;" as "&amp;A11&amp;","</f>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as engagements,</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>engagements as engagements,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f>C12&amp;" as "&amp;A12&amp;","</f>
+      <c r="D13" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>imps as impressions,</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>impressions as impressions,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f>C13&amp;" as "&amp;A13&amp;","</f>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as installs,</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as installs,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f>C14&amp;" as "&amp;A14&amp;","</f>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as likes,</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>likes as likes,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f>C15&amp;" as "&amp;A15&amp;","</f>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as link_clicks,</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>url_clicks as link_clicks,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="str">
-        <f>C16&amp;" as "&amp;A16&amp;","</f>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>NULL as placement_id,</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>NULL as placement_id,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f>C17&amp;" as "&amp;A17&amp;","</f>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as post_click_conversions,</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as post_click_conversions,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f>C18&amp;" as "&amp;A18&amp;","</f>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as post_view_conversions,</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as post_view_conversions,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f>C19&amp;" as "&amp;A19&amp;","</f>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as posts,</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as posts,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f>C20&amp;" as "&amp;A20&amp;","</f>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as purchase,</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as purchase,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f>C21&amp;" as "&amp;A21&amp;","</f>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as registrations,</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as registrations,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="2" t="str">
-        <f>C22&amp;" as "&amp;A22&amp;","</f>
+      <c r="D23" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>revenue as revenue,</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as revenue,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f>C23&amp;" as "&amp;A23&amp;","</f>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as shares,</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as shares,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="2" t="str">
-        <f>C24&amp;" as "&amp;A24&amp;","</f>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>spend as spend,</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>spend as spend,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="2" t="str">
-        <f>C25&amp;" as "&amp;A25&amp;","</f>
+      <c r="D26" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>conv as total_conversions,</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0 as total_conversions,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="str">
-        <f>C26&amp;" as "&amp;A26&amp;","</f>
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>0 as video_views,</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>video_total_views as video_views,</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>